<commit_message>
Stood up most of the helper functions to automate file metadata collection
</commit_message>
<xml_diff>
--- a/Supporting documents/DatabaseModel.xlsx
+++ b/Supporting documents/DatabaseModel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Code\Briel comics website\briel-comics\Supporting documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A82E4B4-C1C7-4F87-B27E-71375AAF544F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC723C87-B8AD-41E8-B02C-4C4AC7B1F3EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6920" yWindow="0" windowWidth="12370" windowHeight="10890" xr2:uid="{62842339-F541-468E-8E69-C4F2980B3155}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{62842339-F541-468E-8E69-C4F2980B3155}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="45">
   <si>
     <t>File ID</t>
   </si>
@@ -141,6 +141,36 @@
   </si>
   <si>
     <t>Tag name table</t>
+  </si>
+  <si>
+    <t>Associated files</t>
+  </si>
+  <si>
+    <t>Previous page ID</t>
+  </si>
+  <si>
+    <t>Next page ID</t>
+  </si>
+  <si>
+    <t>Associated update</t>
+  </si>
+  <si>
+    <t>Page number in associated update</t>
+  </si>
+  <si>
+    <t>Previous update</t>
+  </si>
+  <si>
+    <t>Next update</t>
+  </si>
+  <si>
+    <t>Date posted</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>Content warnings</t>
   </si>
 </sst>
 </file>
@@ -249,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -259,7 +289,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -596,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CE2F903-82D0-4D8A-AEEB-5CCCDA1E54FD}">
   <dimension ref="B2:Q44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -612,12 +641,14 @@
     <col min="8" max="8" width="16.81640625" customWidth="1"/>
     <col min="9" max="9" width="8.81640625" customWidth="1"/>
     <col min="10" max="10" width="16.08984375" customWidth="1"/>
+    <col min="11" max="11" width="14.453125" customWidth="1"/>
     <col min="12" max="12" width="10.1796875" customWidth="1"/>
+    <col min="14" max="14" width="28.81640625" customWidth="1"/>
     <col min="16" max="16" width="17.54296875" customWidth="1"/>
     <col min="18" max="18" width="19.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>17</v>
       </c>
@@ -625,12 +656,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="9"/>
       <c r="E3" s="1" t="s">
         <v>27</v>
       </c>
@@ -638,13 +668,15 @@
         <v>20</v>
       </c>
       <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="K3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="9"/>
       <c r="E4" s="5" t="s">
         <v>28</v>
       </c>
@@ -653,13 +685,19 @@
         <v>21</v>
       </c>
       <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2"/>
+      <c r="N4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="9"/>
       <c r="E5" s="8" t="s">
         <v>3</v>
       </c>
@@ -668,33 +706,54 @@
         <v>22</v>
       </c>
       <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="K5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" s="3"/>
+      <c r="N5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" s="2"/>
+    </row>
+    <row r="6" spans="2:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B6" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="9"/>
-    </row>
-    <row r="7" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" s="3"/>
+      <c r="N6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O6" s="3"/>
+    </row>
+    <row r="7" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="9"/>
       <c r="E7" s="1" t="s">
         <v>34</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="K7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="3"/>
+      <c r="N7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="O7" s="3"/>
+    </row>
+    <row r="8" spans="2:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B8" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="9"/>
       <c r="E8" s="5" t="s">
         <v>28</v>
       </c>
@@ -703,13 +762,20 @@
         <v>20</v>
       </c>
       <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L8" s="3"/>
+      <c r="N8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="O8" s="3"/>
+    </row>
+    <row r="9" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="9"/>
       <c r="E9" s="7" t="s">
         <v>29</v>
       </c>
@@ -718,30 +784,51 @@
         <v>3</v>
       </c>
       <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="K9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L9" s="3"/>
+      <c r="N9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="O9" s="3"/>
+    </row>
+    <row r="10" spans="2:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B10" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="9"/>
-    </row>
-    <row r="11" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L10" s="3"/>
+      <c r="N10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="O10" s="3"/>
+    </row>
+    <row r="11" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="3"/>
-      <c r="D11" s="9"/>
       <c r="H11" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="2:9" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L11" s="3"/>
+      <c r="N11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="O11" s="3"/>
+    </row>
+    <row r="12" spans="2:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="9"/>
       <c r="E12" s="1" t="s">
         <v>30</v>
       </c>
@@ -749,8 +836,16 @@
         <v>24</v>
       </c>
       <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="2:9" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L12" s="4"/>
+      <c r="N12" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O12" s="3"/>
+    </row>
+    <row r="13" spans="2:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E13" s="5" t="s">
         <v>32</v>
       </c>
@@ -759,19 +854,31 @@
         <v>25</v>
       </c>
       <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="2:9" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N13" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O13" s="3"/>
+    </row>
+    <row r="14" spans="2:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E14" s="8" t="s">
         <v>3</v>
       </c>
       <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="2:9" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O14" s="3"/>
+    </row>
+    <row r="15" spans="2:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="2:9" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="2:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B16" s="5" t="s">
         <v>3</v>
       </c>
@@ -779,8 +886,12 @@
       <c r="E16" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="N16" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="O16" s="3"/>
+    </row>
+    <row r="17" spans="2:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B17" s="6" t="s">
         <v>10</v>
       </c>
@@ -789,8 +900,12 @@
         <v>32</v>
       </c>
       <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N17" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="O17" s="3"/>
+    </row>
+    <row r="18" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B18" s="6" t="s">
         <v>12</v>
       </c>
@@ -799,38 +914,42 @@
         <v>33</v>
       </c>
       <c r="F18" s="4"/>
-    </row>
-    <row r="19" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="N18" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="O18" s="4"/>
+    </row>
+    <row r="19" spans="2:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B19" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B20" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:15" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B22" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B23" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B24" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="2:15" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="41" spans="16:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="P41" s="1"/>
     </row>

</xml_diff>